<commit_message>
✨ Feat : DND 기능 개발
</commit_message>
<xml_diff>
--- a/project/public/file/bulk-input-data.xlsx
+++ b/project/public/file/bulk-input-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m3088\OneDrive\바탕 화면\　\코딩\My\프로젝트\V-DAS\project\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF9B4F3-B823-488D-9452-B71EEFF8CEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A6064D-3ED5-4E43-B9A2-1BC7D8AFE6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{2C90205A-45B4-C04B-97C1-2FDE7A5BDBE6}"/>
+    <workbookView xWindow="13920" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{2C90205A-45B4-C04B-97C1-2FDE7A5BDBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="DB변환" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7820ECB5-0782-0B42-B43D-4277CF5933AB}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>